<commit_message>
[test] edit miappe template, remove example values
</commit_message>
<xml_diff>
--- a/templates/community/test_Stella/MIAPPE_biological_material_observation_unit_new.xlsx
+++ b/templates/community/test_Stella/MIAPPE_biological_material_observation_unit_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\sciebo - Eggels, Stella (s.eggels@fz-juelich.de)@fz-juelich.sciebo.de\SE\DataPLANT\ARCs und SWATE\Ersatz fehlerhafter MIAPPE templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/Swate-templates/templates/community/test_Stella/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BC7C0A-CB4C-463F-9600-2AD845AFE544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7040B8A0-2209-2C49-A01A-964AA5DA4491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-96" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0F33DF36-A4CC-4604-A18D-61BD077FEF27}"/>
+    <workbookView xWindow="940" yWindow="500" windowWidth="27860" windowHeight="17500" activeTab="1" xr2:uid="{0F33DF36-A4CC-4604-A18D-61BD077FEF27}"/>
   </bookViews>
   <sheets>
     <sheet name="biological_material" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -52,76 +51,157 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{BA857457-6657-4AD9-9A12-7B91CF5D6D2C}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The unique identifier of this template. It will be auto generated.
 Reply:
     id=0695f30b-e3d7-4c6b-b3c2-4ebdccab8670</t>
+        </r>
       </text>
     </comment>
     <comment ref="A2" authorId="1" shapeId="0" xr:uid="{142D07E3-1D68-4EA5-BB08-9050165A9D5A}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The name of the Swate template.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A3" authorId="2" shapeId="0" xr:uid="{984EEE78-EC91-41FA-89C1-54B1ACF4B37E}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The current version of this template in SemVer notation.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A4" authorId="3" shapeId="0" xr:uid="{E50B3694-F660-4066-A2B0-4AC4AE0739A1}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The description of this template. Use few sentences for succinctness.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A5" authorId="4" shapeId="0" xr:uid="{969A7CEA-0B3F-45B0-ABA0-FBE11E9E0743}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A6" authorId="5" shapeId="0" xr:uid="{396D65E8-ED4C-45AB-8957-B9A86D3CC59F}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The name of the Swate annotation table in the workbook of the template's excel file.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A7" authorId="6" shapeId="0" xr:uid="{59ADA713-4A64-477C-9FE5-89A5A03E0EBD}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A11" authorId="7" shapeId="0" xr:uid="{2050CBDC-7534-48DC-9B0B-6A9AFF86215E}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     A list of all tags associated with this template. Tags are realized as Terms.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A15" authorId="8" shapeId="0" xr:uid="{DB5666DC-4F86-41EF-8B55-C65D3B271F02}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The author(s) of this template.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -129,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="105">
   <si>
     <t>Source Name</t>
   </si>
@@ -224,9 +304,6 @@
     <t>Characteristic [Organism]</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Term Source REF (MIAPPE:0041)</t>
   </si>
   <si>
@@ -395,157 +472,12 @@
     <t>Term Accession Number (MIAPPE:0073)</t>
   </si>
   <si>
-    <t xml:space="preserve">An identifier for the organism at the species level. Use of the NCBI taxon ID is recommended. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NCBITAXON:4577 </t>
-  </si>
-  <si>
-    <t>Unique identifier</t>
-  </si>
-  <si>
-    <t>Genus name for the organism under study, according to standard scientific nomenclature.</t>
-  </si>
-  <si>
-    <t>Genus name</t>
-  </si>
-  <si>
-    <t>Species name</t>
-  </si>
-  <si>
-    <t>Name of any subtaxa level, including variety, crossing name, etc. It can be used to store any additional taxonomic identifier. Either free text description or key-value pair list format (the key is the name of the rank and the value is the value of  the rank). Ranks can be among the following terms: subspecies, cultivar, variety, subvariety, convariety, group, subgroup, hybrid, line, form, subform. For MCPD compliance, the following abbreviations are allowed: ‘subsp.’ (subspecies); ‘convar.’ (convariety); ‘var.’ (variety); ‘f.’ (form); ‘Group’ (cultivar group).</t>
-  </si>
-  <si>
-    <t>vinifera Pinot noir
-B73
-subspecies:vinifera ; cultivar:Pinot noir
-var:B73
-subsp. vinifera var. Pinot Noir
-var. B73</t>
-  </si>
-  <si>
-    <t>Free text, or key-value pair list, or MCPD-compliant format</t>
-  </si>
-  <si>
-    <t>Species name (formally: specific epithet) for the organism under study, according to standard scientific nomenclature.</t>
-  </si>
-  <si>
-    <t>mays
-lycosperium x pennellii</t>
-  </si>
-  <si>
-    <t>Zea
-Solanum</t>
-  </si>
-  <si>
-    <t>Latitude of the studied biological material. [Alternative identifier for in situ material]</t>
-  </si>
-  <si>
-    <t>+39.067</t>
-  </si>
-  <si>
-    <t>Degrees in the decimal format (ISO 6709)</t>
-  </si>
-  <si>
-    <t>Longitude of the studied biological material. [Alternative identifier for in situ material]</t>
-  </si>
-  <si>
-    <t>Altitude of the studied biological material, provided in meters (m). [Alternative identifier for in situ material]</t>
-  </si>
-  <si>
-    <t>10 m</t>
-  </si>
-  <si>
-    <t>Numeric + unit abbreviation</t>
-  </si>
-  <si>
-    <t>Circular uncertainty of the coordinates, preferably provided in meters (m). [Alternative identifier for in situ material]</t>
-  </si>
-  <si>
-    <t>200 m</t>
-  </si>
-  <si>
-    <t>Numeric</t>
-  </si>
-  <si>
-    <t>Description of any process or treatment applied uniformly to the biological material, prior to the study itself. Can be provided as free text or as an accession number from a suitable controlled vocabulary.</t>
-  </si>
-  <si>
-    <t>EO:0007210 - PVY(NTN); transplanted from study http://phenome-fppn.fr/maugio/2013/t2351 observation unit ID: pot:894</t>
-  </si>
-  <si>
-    <t>Plant Environment Ontology and/or free text</t>
-  </si>
-  <si>
-    <t>An identifier for the source of the biological material, in the form of a key-value pair comprising the name/identifier of the repository from which the material was sourced plus the accession number of the repository for that material. Where an accession number has not been assigned, but the material has been derived from the crossing of known accessions, the material can be defined as follows: "mother_accession X father_accession", or, if father is unknown, as "mother_accession X UNKNOWN". For in situ material, the region of provenance may be used when an accession is not available.</t>
-  </si>
-  <si>
-    <t>INRA:W95115_inra
-ICNF:PNB-RPI</t>
-  </si>
-  <si>
-    <t>Digital Object Identifier (DOI) of the material source</t>
-  </si>
-  <si>
-    <t>doi:10.15454/1.4658436467893904E12</t>
-  </si>
-  <si>
-    <t>DOI</t>
-  </si>
-  <si>
-    <t>Latitude of the material source. [Alternative identifier for in situ material]</t>
-  </si>
-  <si>
-    <t>Longitude of the material source. [Alternative identifier for in situ material]</t>
-  </si>
-  <si>
-    <t>Altitude of the material source, provided in metres (m). [Alternative identifier for in situ material]</t>
-  </si>
-  <si>
-    <t>Circular uncertainty of the coordinates, provided in meters (m). [Alternative identifier for in situ material]</t>
-  </si>
-  <si>
-    <t>Description of the material source</t>
-  </si>
-  <si>
-    <t>Branches were collected from a 10-year-old tree growing in a progeny trial established in a loamy brown earth soil.</t>
-  </si>
-  <si>
-    <t>Free text</t>
-  </si>
-  <si>
-    <t>Type of observation unit in textual form, usually one of the following: study, block, sub-block, plot, sub-plot, pot, plant. Use of other observation unit types is possible but not recommended. 
-The observation unit type cannot be used to indicate sub-plant levels. However, observations can still be made on the sub-plant level, as long as the details are indicated in the associated observed variable (see observed variables).
-Alternatively, it is possible to use samples for more detailed tracing of sub-plant units, attaching the observations to them instead.</t>
-  </si>
-  <si>
-    <t>plot</t>
-  </si>
-  <si>
-    <t>Identifier for the observation unit in a persistent repository, comprises the name of the repository and the identifier of the observation unit therein. The EBI Biosamples repository can be used. URI are recommended when possible.</t>
-  </si>
-  <si>
-    <t>Biosamples:SAMEA4202911</t>
-  </si>
-  <si>
-    <t>Type and value of a spatial coordinate (georeference or relative) or level of observation (plot 45, subblock 7, block 2) provided as a key-value pair of the form type:value. Levels of observation must be consistent with those listed in the Study section.</t>
-  </si>
-  <si>
-    <t>latitude:+2.341; row:4 ; X:3; Y:6; Xm:35; Ym:65; block:1; plot:894</t>
-  </si>
-  <si>
-    <t>Formatted text (Key:value)</t>
-  </si>
-  <si>
     <t>MIAPPE biological material</t>
   </si>
   <si>
     <t>Template to describe the biological material and observation unit according to MIAPPE v.1.1.</t>
   </si>
   <si>
-    <t>1.0.1</t>
-  </si>
-  <si>
     <t>DataPLANT</t>
   </si>
   <si>
@@ -589,6 +521,9 @@
   </si>
   <si>
     <t>s.eggels@fz-juelich.de</t>
+  </si>
+  <si>
+    <t>1.0.2</t>
   </si>
 </sst>
 </file>
@@ -742,7 +677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -778,9 +713,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1111,8 +1043,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{322D68E6-1FA7-470F-A94D-B3975DBF0DB4}" name="annotationTableHorribleMonkey23" displayName="annotationTableHorribleMonkey23" ref="A1:BG4" totalsRowShown="0">
-  <autoFilter ref="A1:BG4" xr:uid="{322D68E6-1FA7-470F-A94D-B3975DBF0DB4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{322D68E6-1FA7-470F-A94D-B3975DBF0DB4}" name="annotationTableHorribleMonkey23" displayName="annotationTableHorribleMonkey23" ref="A1:BG2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:BG2" xr:uid="{322D68E6-1FA7-470F-A94D-B3975DBF0DB4}"/>
   <tableColumns count="59">
     <tableColumn id="1" xr3:uid="{FE826609-98EA-44A1-99F7-EB3AAEFDF050}" name="Source Name"/>
     <tableColumn id="3" xr3:uid="{1BEB5726-5F75-4B01-A0AB-AAB8F1E15FC9}" name="Characteristic [Organism]" dataDxfId="56"/>
@@ -1528,72 +1460,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334B6C2A-9207-4051-9C31-3F62AC75BDC7}">
-  <dimension ref="A1:BG4"/>
+  <dimension ref="A1:BG2"/>
   <sheetViews>
-    <sheetView topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="AR5" sqref="AR5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="37.33203125" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="39.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="40.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="39.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="53.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="53.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="37.33203125" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="67.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="68.77734375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="68.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="37.33203125" hidden="1" customWidth="1"/>
     <col min="32" max="32" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="34" max="34" width="37.33203125" hidden="1" customWidth="1"/>
     <col min="35" max="35" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="37" max="37" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="38.77734375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="36.83203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="43" max="43" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="50.77734375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="30.83203125" hidden="1" customWidth="1"/>
     <col min="46" max="46" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="39.77734375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="48" max="49" width="0" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="35.1640625" bestFit="1" customWidth="1"/>
     <col min="51" max="52" width="0" hidden="1" customWidth="1"/>
     <col min="53" max="53" width="32" bestFit="1" customWidth="1"/>
     <col min="54" max="55" width="0" hidden="1" customWidth="1"/>
     <col min="56" max="56" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="57" max="58" width="0" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1601,575 +1531,235 @@
         <v>30</v>
       </c>
       <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>41</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>42</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>43</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>44</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>46</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>47</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>48</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>49</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>50</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>51</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>52</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>53</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>54</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>55</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>56</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>58</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>59</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>60</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>61</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>62</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>63</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>64</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>65</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>66</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>67</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>68</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>69</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>70</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>71</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>72</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>73</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>74</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>75</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>76</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>77</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>78</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>79</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>80</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>81</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>82</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>83</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>84</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>85</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>86</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>87</v>
       </c>
       <c r="BG1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:59" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="V2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="W2" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z2" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC2" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF2" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI2" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="AJ2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL2" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AO2" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AQ2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AR2" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="AS2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AT2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AU2" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="AV2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AW2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AX2" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="AY2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AZ2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="BA2" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="BB2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="BC2" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="BD2" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="BE2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="BF2" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:59" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11">
-        <v>-8.73</v>
-      </c>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="U3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="V3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="W3" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="X3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z3" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="AD3" s="11"/>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG3" s="11"/>
-      <c r="AH3" s="11"/>
-      <c r="AI3" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="AJ3" s="11"/>
-      <c r="AK3" s="11"/>
-      <c r="AL3" s="11">
-        <v>-8.73</v>
-      </c>
-      <c r="AM3" s="11"/>
-      <c r="AN3" s="11"/>
-      <c r="AO3" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="AP3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AQ3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AR3" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="AS3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AT3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AU3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="AV3" s="11"/>
-      <c r="AW3" s="11"/>
-      <c r="AX3" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="AY3" s="11"/>
-      <c r="AZ3" s="11"/>
-      <c r="BA3" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="BB3" s="11"/>
-      <c r="BC3" s="11"/>
-      <c r="BD3" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="BE3" s="10"/>
-      <c r="BF3" s="10"/>
-    </row>
-    <row r="4" spans="1:59" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="U4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="V4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="W4" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="X4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z4" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA4" s="11"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG4" s="11"/>
-      <c r="AH4" s="11"/>
-      <c r="AI4" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="AJ4" s="11"/>
-      <c r="AK4" s="11"/>
-      <c r="AL4" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="AM4" s="11"/>
-      <c r="AN4" s="11"/>
-      <c r="AO4" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="AP4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AQ4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AR4" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="AS4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AT4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AU4" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="AV4" s="11"/>
-      <c r="AW4" s="11"/>
-      <c r="AX4" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="AY4" s="11"/>
-      <c r="AZ4" s="11"/>
-      <c r="BA4" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="BB4" s="11"/>
-      <c r="BC4" s="11"/>
-      <c r="BD4" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="BE4" s="10"/>
-      <c r="BF4" s="10"/>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
+      <c r="B2" s="11"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="11"/>
+      <c r="AJ2" s="11"/>
+      <c r="AK2" s="11"/>
+      <c r="AL2" s="11"/>
+      <c r="AM2" s="11"/>
+      <c r="AN2" s="11"/>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="11"/>
+      <c r="AQ2" s="11"/>
+      <c r="AR2" s="11"/>
+      <c r="AS2" s="11"/>
+      <c r="AT2" s="11"/>
+      <c r="AU2" s="11"/>
+      <c r="AV2" s="11"/>
+      <c r="AW2" s="11"/>
+      <c r="AX2" s="11"/>
+      <c r="AY2" s="11"/>
+      <c r="AZ2" s="11"/>
+      <c r="BA2" s="11"/>
+      <c r="BB2" s="11"/>
+      <c r="BC2" s="11"/>
+      <c r="BD2" s="11"/>
+      <c r="BE2" s="10"/>
+      <c r="BF2" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2184,17 +1774,17 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.5" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2202,207 +1792,207 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>138</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="D16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>

</xml_diff>